<commit_message>
adding new text to resources page
</commit_message>
<xml_diff>
--- a/data/IMN-textfiles/Districts_New-Old.xlsx
+++ b/data/IMN-textfiles/Districts_New-Old.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>OLD</t>
   </si>
@@ -50,6 +50,99 @@
   </si>
   <si>
     <t>N4</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>N6</t>
+  </si>
+  <si>
+    <t>N7</t>
+  </si>
+  <si>
+    <t>N8</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
@@ -81,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,14 +182,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,55 +522,250 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="F2"/>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C34" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created write to excel button and function
</commit_message>
<xml_diff>
--- a/data/IMN-textfiles/Districts_New-Old.xlsx
+++ b/data/IMN-textfiles/Districts_New-Old.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>OLD</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>S2</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>E10 part</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>W3</t>
   </si>
 </sst>
 </file>
@@ -514,7 +526,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +549,9 @@
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F2"/>
       <c r="G2"/>
     </row>
@@ -547,24 +562,42 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -626,37 +659,37 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -664,7 +697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
@@ -672,55 +705,60 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
updates to excel compare script
</commit_message>
<xml_diff>
--- a/data/IMN-textfiles/Districts_New-Old.xlsx
+++ b/data/IMN-textfiles/Districts_New-Old.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>OLD</t>
   </si>
@@ -151,10 +151,55 @@
     <t>E10 part</t>
   </si>
   <si>
-    <t>skip</t>
-  </si>
-  <si>
     <t>W3</t>
+  </si>
+  <si>
+    <t>skip, thin and long, east west</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>W6</t>
+  </si>
+  <si>
+    <t>W8</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>W7</t>
+  </si>
+  <si>
+    <t>W4</t>
+  </si>
+  <si>
+    <t>E1 &amp; E3</t>
+  </si>
+  <si>
+    <t>S6, S4</t>
+  </si>
+  <si>
+    <t>S2, S4</t>
+  </si>
+  <si>
+    <t>wip</t>
   </si>
 </sst>
 </file>
@@ -213,12 +258,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +572,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +595,7 @@
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F2"/>
@@ -574,7 +620,7 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -604,90 +650,148 @@
         <v>15</v>
       </c>
       <c r="C7" s="4"/>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -710,7 +814,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
@@ -720,55 +824,73 @@
       <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -782,25 +904,33 @@
       <c r="B35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added color codes to priorities
</commit_message>
<xml_diff>
--- a/data/IMN-textfiles/Districts_New-Old.xlsx
+++ b/data/IMN-textfiles/Districts_New-Old.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>OLD</t>
   </si>
@@ -148,15 +148,9 @@
     <t>done</t>
   </si>
   <si>
-    <t>E10 part</t>
-  </si>
-  <si>
     <t>W3</t>
   </si>
   <si>
-    <t>skip, thin and long, east west</t>
-  </si>
-  <si>
     <t>E7</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>W4</t>
   </si>
   <si>
-    <t>E1 &amp; E3</t>
-  </si>
-  <si>
     <t>S6, S4</t>
   </si>
   <si>
@@ -200,6 +191,18 @@
   </si>
   <si>
     <t>wip</t>
+  </si>
+  <si>
+    <t>N1 &amp; W4</t>
+  </si>
+  <si>
+    <t>part W5</t>
+  </si>
+  <si>
+    <t>E1 &amp; E3, no E3 writeup</t>
+  </si>
+  <si>
+    <t>E10 but no writeup</t>
   </si>
 </sst>
 </file>
@@ -571,13 +574,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
@@ -617,10 +621,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -692,7 +696,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -703,7 +707,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
         <v>43</v>
@@ -714,7 +718,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
         <v>43</v>
@@ -725,7 +729,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -736,7 +740,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -747,10 +751,10 @@
         <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -760,13 +764,19 @@
       <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -774,7 +784,10 @@
         <v>27</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -782,7 +795,10 @@
         <v>28</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -790,7 +806,10 @@
         <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -800,6 +819,9 @@
       <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -808,13 +830,16 @@
       <c r="C23" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
@@ -825,7 +850,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -833,7 +861,10 @@
         <v>31</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -841,7 +872,10 @@
         <v>32</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -851,13 +885,19 @@
       <c r="C28" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -865,6 +905,9 @@
         <v>41</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
         <v>58</v>
       </c>
     </row>
@@ -913,7 +956,7 @@
         <v>38</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -921,7 +964,7 @@
         <v>39</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added enforcement by jurisdiction
</commit_message>
<xml_diff>
--- a/data/IMN-textfiles/Districts_New-Old.xlsx
+++ b/data/IMN-textfiles/Districts_New-Old.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
   <si>
     <t>OLD</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>E10 but no writeup</t>
+  </si>
+  <si>
+    <t>S7 &amp; S8</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
   <dimension ref="B1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +627,7 @@
         <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -908,7 +911,7 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -918,6 +921,9 @@
       <c r="C31" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -926,16 +932,22 @@
       <c r="C32" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>5</v>
       </c>
@@ -943,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>37</v>
       </c>
@@ -951,7 +963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>38</v>
       </c>
@@ -959,7 +971,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>39</v>
       </c>
@@ -967,7 +979,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>